<commit_message>
Fix illegal memory access
</commit_message>
<xml_diff>
--- a/scripts/Experiment 1 Results/Experiment 1 Graphs.xlsx
+++ b/scripts/Experiment 1 Results/Experiment 1 Graphs.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17600" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Exp1, w=10" sheetId="1" r:id="rId1"/>
@@ -27,17 +27,14 @@
     <definedName name="Exp1_ABT_loss_0.6_1" localSheetId="1">'Exp1, w=50'!$L$45:$V$55</definedName>
     <definedName name="Exp1_ABT_loss_0.8" localSheetId="0">'Exp1, w=10'!$E$86:$O$96</definedName>
     <definedName name="Exp1_ABT_loss_0.8_1" localSheetId="1">'Exp1, w=50'!$A$86:$K$96</definedName>
-    <definedName name="Exp1_GBN_loss_0.1_window_10" localSheetId="0">'Exp1, w=10'!$E$17:$O$27</definedName>
+    <definedName name="Exp1_GBN_loss_0.1_window_10_1" localSheetId="0">'Exp1, w=10'!$E$17:$O$27</definedName>
     <definedName name="Exp1_GBN_loss_0.1_window_50" localSheetId="1">'Exp1, w=50'!$A$17:$K$27</definedName>
-    <definedName name="Exp1_GBN_loss_0.2_window_10" localSheetId="0">'Exp1, w=10'!$P$17:$Z$27</definedName>
+    <definedName name="Exp1_GBN_loss_0.2_window_10_1" localSheetId="0">'Exp1, w=10'!$P$17:$Z$25</definedName>
     <definedName name="Exp1_GBN_loss_0.2_window_50" localSheetId="1">'Exp1, w=50'!$L$17:$V$27</definedName>
     <definedName name="Exp1_GBN_loss_0.2_window_50_1" localSheetId="1">'Exp1, w=50'!$L$30:$V$40</definedName>
-    <definedName name="Exp1_GBN_loss_0.4_window_10" localSheetId="0">'Exp1, w=10'!$E$58:$O$68</definedName>
     <definedName name="Exp1_GBN_loss_0.4_window_10_1" localSheetId="0">'Exp1, w=10'!$E$71:$O$81</definedName>
     <definedName name="Exp1_GBN_loss_0.4_window_50" localSheetId="1">'Exp1, w=50'!$A$58:$K$68</definedName>
-    <definedName name="Exp1_GBN_loss_0.6_window_10" localSheetId="0">'Exp1, w=10'!$P$58:$Z$68</definedName>
     <definedName name="Exp1_GBN_loss_0.6_window_50" localSheetId="1">'Exp1, w=50'!$L$58:$V$68</definedName>
-    <definedName name="Exp1_GBN_loss_0.8_window_10" localSheetId="0">'Exp1, w=10'!$E$99:$O$109</definedName>
     <definedName name="Exp1_GBN_loss_0.8_window_10_1" localSheetId="0">'Exp1, w=10'!$E$112:$O$122</definedName>
     <definedName name="Exp1_GBN_loss_0.8_window_50" localSheetId="1">'Exp1, w=50'!$A$99:$K$109</definedName>
     <definedName name="Exp1_SR_loss_0.1_window_10_1" localSheetId="0">'Exp1, w=10'!$E$30:$O$40</definedName>
@@ -140,18 +137,8 @@
     </textPr>
   </connection>
   <connection id="11" name="Exp1-GBN-loss-0.1-window-10" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" codePage="10000" sourceFile="/Users/Bobby/Desktop/Spring 2016/CSE489/Assignments/ReliableTransportProtocols/scripts/Experiment 1 Results/Exp1-GBN-loss-0.1-window-10.csv" comma="1">
-      <textFields count="11">
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
+    <textPr fileType="mac" codePage="10000" sourceFile="/Users/Bobby/Desktop/Spring 2016/CSE489/Assignments/ReliableTransportProtocols/scripts/Exp1-GBN-loss-0.1-window-10.csv" comma="1">
+      <textFields>
         <textField/>
       </textFields>
     </textPr>
@@ -164,7 +151,7 @@
     </textPr>
   </connection>
   <connection id="13" name="Exp1-GBN-loss-0.2-window-10" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" codePage="10000" sourceFile="/Users/Bobby/Desktop/Spring 2016/CSE489/Assignments/ReliableTransportProtocols/scripts/Experiment 1 Results/Exp1-GBN-loss-0.2-window-10.csv" comma="1">
+    <textPr fileType="mac" codePage="10000" sourceFile="/Users/Bobby/Desktop/Spring 2016/CSE489/Assignments/ReliableTransportProtocols/scripts/Exp1-GBN-loss-0.2-window-10.csv" comma="1">
       <textFields>
         <textField/>
       </textFields>
@@ -184,105 +171,84 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="16" name="Exp1-GBN-loss-0.4-window-10" type="6" refreshedVersion="0" background="1" saveData="1">
+  <connection id="16" name="Exp1-GBN-loss-0.4-window-101" type="6" refreshedVersion="0" background="1" saveData="1">
     <textPr fileType="mac" codePage="10000" sourceFile="/Users/Bobby/Desktop/Spring 2016/CSE489/Assignments/ReliableTransportProtocols/scripts/Experiment 1 Results/Exp1-GBN-loss-0.4-window-10.csv" comma="1">
       <textFields>
         <textField/>
       </textFields>
     </textPr>
   </connection>
-  <connection id="17" name="Exp1-GBN-loss-0.4-window-101" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" codePage="10000" sourceFile="/Users/Bobby/Desktop/Spring 2016/CSE489/Assignments/ReliableTransportProtocols/scripts/Experiment 1 Results/Exp1-GBN-loss-0.4-window-10.csv" comma="1">
-      <textFields>
-        <textField/>
-      </textFields>
-    </textPr>
-  </connection>
-  <connection id="18" name="Exp1-GBN-loss-0.4-window-50" type="6" refreshedVersion="0" background="1" saveData="1">
+  <connection id="17" name="Exp1-GBN-loss-0.4-window-50" type="6" refreshedVersion="0" background="1" saveData="1">
     <textPr fileType="mac" codePage="10000" sourceFile="/Users/Bobby/Desktop/Spring 2016/CSE489/Assignments/ReliableTransportProtocols/scripts/Experiment 1 Results/Exp1-GBN-loss-0.4-window-50.csv" comma="1">
       <textFields>
         <textField/>
       </textFields>
     </textPr>
   </connection>
-  <connection id="19" name="Exp1-GBN-loss-0.6-window-10" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" codePage="10000" sourceFile="/Users/Bobby/Desktop/Spring 2016/CSE489/Assignments/ReliableTransportProtocols/scripts/Experiment 1 Results/Exp1-GBN-loss-0.6-window-10.csv" comma="1">
-      <textFields>
-        <textField/>
-      </textFields>
-    </textPr>
-  </connection>
-  <connection id="20" name="Exp1-GBN-loss-0.6-window-50" type="6" refreshedVersion="0" background="1" saveData="1">
+  <connection id="18" name="Exp1-GBN-loss-0.6-window-50" type="6" refreshedVersion="0" background="1" saveData="1">
     <textPr fileType="mac" codePage="10000" sourceFile="/Users/Bobby/Desktop/Spring 2016/CSE489/Assignments/ReliableTransportProtocols/scripts/Experiment 1 Results/Exp1-GBN-loss-0.6-window-50.csv" comma="1">
       <textFields>
         <textField/>
       </textFields>
     </textPr>
   </connection>
-  <connection id="21" name="Exp1-GBN-loss-0.8-window-10" type="6" refreshedVersion="0" background="1" saveData="1">
+  <connection id="19" name="Exp1-GBN-loss-0.8-window-101" type="6" refreshedVersion="0" background="1" saveData="1">
     <textPr fileType="mac" codePage="10000" sourceFile="/Users/Bobby/Desktop/Spring 2016/CSE489/Assignments/ReliableTransportProtocols/scripts/Experiment 1 Results/Exp1-GBN-loss-0.8-window-10.csv" comma="1">
       <textFields>
         <textField/>
       </textFields>
     </textPr>
   </connection>
-  <connection id="22" name="Exp1-GBN-loss-0.8-window-101" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" codePage="10000" sourceFile="/Users/Bobby/Desktop/Spring 2016/CSE489/Assignments/ReliableTransportProtocols/scripts/Experiment 1 Results/Exp1-GBN-loss-0.8-window-10.csv" comma="1">
-      <textFields>
-        <textField/>
-      </textFields>
-    </textPr>
-  </connection>
-  <connection id="23" name="Exp1-GBN-loss-0.8-window-50" type="6" refreshedVersion="0" background="1" saveData="1">
+  <connection id="20" name="Exp1-GBN-loss-0.8-window-50" type="6" refreshedVersion="0" background="1" saveData="1">
     <textPr fileType="mac" codePage="10000" sourceFile="/Users/Bobby/Desktop/Spring 2016/CSE489/Assignments/ReliableTransportProtocols/scripts/Experiment 1 Results/Exp1-GBN-loss-0.8-window-50.csv" comma="1">
       <textFields>
         <textField/>
       </textFields>
     </textPr>
   </connection>
-  <connection id="24" name="Exp1-SR-loss-0.1-window-10" type="6" refreshedVersion="0" background="1" saveData="1">
+  <connection id="21" name="Exp1-SR-loss-0.1-window-10" type="6" refreshedVersion="0" background="1" saveData="1">
     <textPr fileType="mac" codePage="10000" sourceFile="/Users/Bobby/Desktop/Spring 2016/CSE489/Assignments/ReliableTransportProtocols/scripts/Experiment 1 Results/Exp1-SR-loss-0.1-window-10.csv" comma="1">
       <textFields>
         <textField/>
       </textFields>
     </textPr>
   </connection>
-  <connection id="25" name="Exp1-SR-loss-0.1-window-50" type="6" refreshedVersion="0" background="1" saveData="1">
+  <connection id="22" name="Exp1-SR-loss-0.1-window-50" type="6" refreshedVersion="0" background="1" saveData="1">
     <textPr fileType="mac" codePage="10000" sourceFile="/Users/Bobby/Desktop/Spring 2016/CSE489/Assignments/ReliableTransportProtocols/scripts/Experiment 1 Results/Exp1-SR-loss-0.1-window-50.csv" comma="1">
       <textFields>
         <textField/>
       </textFields>
     </textPr>
   </connection>
-  <connection id="26" name="Exp1-SR-loss-0.2-window-10" type="6" refreshedVersion="0" background="1" saveData="1">
+  <connection id="23" name="Exp1-SR-loss-0.2-window-10" type="6" refreshedVersion="0" background="1" saveData="1">
     <textPr fileType="mac" codePage="10000" sourceFile="/Users/Bobby/Desktop/Spring 2016/CSE489/Assignments/ReliableTransportProtocols/scripts/Experiment 1 Results/Exp1-SR-loss-0.2-window-10.csv" comma="1">
       <textFields>
         <textField/>
       </textFields>
     </textPr>
   </connection>
-  <connection id="27" name="Exp1-SR-loss-0.4-window-50" type="6" refreshedVersion="0" background="1" saveData="1">
+  <connection id="24" name="Exp1-SR-loss-0.4-window-50" type="6" refreshedVersion="0" background="1" saveData="1">
     <textPr fileType="mac" codePage="10000" sourceFile="/Users/Bobby/Desktop/Spring 2016/CSE489/Assignments/ReliableTransportProtocols/scripts/Experiment 1 Results/Exp1-SR-loss-0.4-window-50.csv" comma="1">
       <textFields>
         <textField/>
       </textFields>
     </textPr>
   </connection>
-  <connection id="28" name="Exp1-SR-loss-0.6-window-10" type="6" refreshedVersion="0" background="1" saveData="1">
+  <connection id="25" name="Exp1-SR-loss-0.6-window-10" type="6" refreshedVersion="0" background="1" saveData="1">
     <textPr fileType="mac" codePage="10000" sourceFile="/Users/Bobby/Desktop/Spring 2016/CSE489/Assignments/ReliableTransportProtocols/scripts/Experiment 1 Results/Exp1-SR-loss-0.6-window-10.csv" comma="1">
       <textFields>
         <textField/>
       </textFields>
     </textPr>
   </connection>
-  <connection id="29" name="Exp1-SR-loss-0.6-window-50" type="6" refreshedVersion="0" background="1" saveData="1">
+  <connection id="26" name="Exp1-SR-loss-0.6-window-50" type="6" refreshedVersion="0" background="1" saveData="1">
     <textPr fileType="mac" codePage="10000" sourceFile="/Users/Bobby/Desktop/Spring 2016/CSE489/Assignments/ReliableTransportProtocols/scripts/Experiment 1 Results/Exp1-SR-loss-0.6-window-50.csv" comma="1">
       <textFields>
         <textField/>
       </textFields>
     </textPr>
   </connection>
-  <connection id="30" name="Exp1-SR-loss-0.8-window-50" type="6" refreshedVersion="0" background="1" saveData="1">
+  <connection id="27" name="Exp1-SR-loss-0.8-window-50" type="6" refreshedVersion="0" background="1" saveData="1">
     <textPr fileType="mac" codePage="10000" sourceFile="/Users/Bobby/Desktop/Spring 2016/CSE489/Assignments/ReliableTransportProtocols/scripts/Experiment 1 Results/Exp1-SR-loss-0.8-window-50.csv" comma="1">
       <textFields>
         <textField/>
@@ -293,7 +259,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="20">
   <si>
     <t>Run</t>
   </si>
@@ -650,119 +616,107 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Exp1-GBN-loss-0.8-window-10_1" connectionId="22" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Exp1-GBN-loss-0.2-window-10_1" connectionId="13" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable10.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Exp1-GBN-loss-0.4-window-10" connectionId="16" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Exp1-ABT-loss-0.4" connectionId="5" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable11.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Exp1-ABT-loss-0.4" connectionId="5" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Exp1-ABT-loss-0.2" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable12.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Exp1-GBN-loss-0.2-window-10" connectionId="13" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Exp1-ABT-loss-0.1" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable13.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Exp1-ABT-loss-0.2" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Exp1-SR-loss-0.8-window-50" connectionId="27" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable14.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Exp1-GBN-loss-0.1-window-10" connectionId="11" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Exp1-GBN-loss-0.8-window-50" connectionId="20" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable15.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Exp1-ABT-loss-0.1" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Exp1-ABT-loss-0.8_1" connectionId="10" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable16.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Exp1-SR-loss-0.8-window-50" connectionId="30" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Exp1-SR-loss-0.6-window-50" connectionId="26" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable17.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Exp1-GBN-loss-0.8-window-50" connectionId="23" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Exp1-GBN-loss-0.6-window-50" connectionId="18" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable18.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Exp1-ABT-loss-0.8_1" connectionId="10" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Exp1-ABT-loss-0.6_1" connectionId="8" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable19.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Exp1-SR-loss-0.6-window-50" connectionId="29" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Exp1-SR-loss-0.4-window-50" connectionId="24" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Exp1-SR-loss-0.6-window-10_1" connectionId="28" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Exp1-GBN-loss-0.1-window-10_1" connectionId="11" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable20.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Exp1-GBN-loss-0.6-window-50" connectionId="20" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Exp1-GBN-loss-0.4-window-50" connectionId="17" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable21.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Exp1-ABT-loss-0.6_1" connectionId="8" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Exp1-ABT-loss-0.4_1" connectionId="6" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable22.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Exp1-SR-loss-0.4-window-50" connectionId="27" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Exp1-GBN-loss-0.2-window-50_1" connectionId="15" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable23.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Exp1-GBN-loss-0.4-window-50" connectionId="18" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Exp1-GBN-loss-0.2-window-50" connectionId="14" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable24.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Exp1-ABT-loss-0.4_1" connectionId="6" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Exp1-ABT-loss-0.2_1" connectionId="4" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable25.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Exp1-GBN-loss-0.2-window-50_1" connectionId="15" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Exp1-SR-loss-0.1-window-50_1" connectionId="22" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable26.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Exp1-GBN-loss-0.2-window-50" connectionId="14" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Exp1-GBN-loss-0.1-window-50" connectionId="12" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable27.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Exp1-ABT-loss-0.2_1" connectionId="4" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable28.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Exp1-SR-loss-0.1-window-50_1" connectionId="25" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable29.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Exp1-GBN-loss-0.1-window-50" connectionId="12" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Exp1-ABT-loss-0.1_1" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Exp1-GBN-loss-0.4-window-10_1" connectionId="17" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable30.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Exp1-ABT-loss-0.1_1" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Exp1-GBN-loss-0.8-window-10_1" connectionId="19" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Exp1-SR-loss-0.2-window-10_1" connectionId="26" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Exp1-SR-loss-0.6-window-10_1" connectionId="25" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Exp1-SR-loss-0.1-window-10_1" connectionId="24" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Exp1-GBN-loss-0.4-window-10_1" connectionId="16" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Exp1-GBN-loss-0.8-window-10" connectionId="21" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Exp1-SR-loss-0.2-window-10_1" connectionId="23" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable7.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Exp1-ABT-loss-0.8" connectionId="9" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Exp1-SR-loss-0.1-window-10_1" connectionId="21" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable8.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Exp1-GBN-loss-0.6-window-10" connectionId="19" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Exp1-ABT-loss-0.8" connectionId="9" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable9.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1034,8 +988,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="E1:Z123"/>
   <sheetViews>
-    <sheetView topLeftCell="B50" zoomScale="83" workbookViewId="0">
-      <selection activeCell="I89" sqref="E1:Z123"/>
+    <sheetView tabSelected="1" zoomScale="83" workbookViewId="0">
+      <selection activeCell="P17" sqref="P17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1044,26 +998,26 @@
     <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="4.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="4.33203125" customWidth="1"/>
-    <col min="6" max="6" width="9" customWidth="1"/>
-    <col min="7" max="7" width="4.5" customWidth="1"/>
-    <col min="8" max="8" width="10" customWidth="1"/>
-    <col min="9" max="9" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.1640625" customWidth="1"/>
-    <col min="15" max="15" width="10.6640625" customWidth="1"/>
+    <col min="5" max="5" width="5" customWidth="1"/>
+    <col min="6" max="6" width="9.1640625" customWidth="1"/>
+    <col min="7" max="7" width="4.83203125" customWidth="1"/>
+    <col min="8" max="8" width="10.1640625" customWidth="1"/>
+    <col min="9" max="9" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.33203125" customWidth="1"/>
+    <col min="15" max="15" width="10.83203125" customWidth="1"/>
     <col min="16" max="16" width="4.33203125" customWidth="1"/>
-    <col min="17" max="17" width="9" customWidth="1"/>
-    <col min="18" max="18" width="4.5" customWidth="1"/>
-    <col min="19" max="19" width="10" customWidth="1"/>
-    <col min="20" max="20" width="17.33203125" customWidth="1"/>
-    <col min="21" max="21" width="12.5" customWidth="1"/>
-    <col min="22" max="23" width="11.1640625" customWidth="1"/>
-    <col min="24" max="24" width="12.33203125" customWidth="1"/>
-    <col min="25" max="25" width="10" customWidth="1"/>
-    <col min="26" max="26" width="10.6640625" customWidth="1"/>
+    <col min="17" max="17" width="9.1640625" customWidth="1"/>
+    <col min="18" max="18" width="4.83203125" customWidth="1"/>
+    <col min="19" max="19" width="10.1640625" customWidth="1"/>
+    <col min="20" max="20" width="17.6640625" customWidth="1"/>
+    <col min="21" max="21" width="12.6640625" customWidth="1"/>
+    <col min="22" max="23" width="11.33203125" customWidth="1"/>
+    <col min="24" max="24" width="12.6640625" customWidth="1"/>
+    <col min="25" max="25" width="12.33203125" customWidth="1"/>
+    <col min="26" max="26" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="5:26" x14ac:dyDescent="0.2">
@@ -2098,19 +2052,19 @@
         <v>1000</v>
       </c>
       <c r="K18" s="2">
-        <v>42773</v>
+        <v>2773</v>
       </c>
       <c r="L18" s="2">
-        <v>9038</v>
+        <v>2484</v>
       </c>
       <c r="M18" s="2">
-        <v>23</v>
+        <v>997</v>
       </c>
       <c r="N18" s="2">
-        <v>49798.664062000003</v>
+        <v>49981.515625</v>
       </c>
       <c r="O18" s="2">
-        <v>4.6200000000000001E-4</v>
+        <v>1.9946999999999999E-2</v>
       </c>
       <c r="P18" s="2">
         <v>1</v>
@@ -2131,19 +2085,19 @@
         <v>1000</v>
       </c>
       <c r="V18" s="2">
-        <v>33998</v>
+        <v>3208</v>
       </c>
       <c r="W18" s="2">
-        <v>9232</v>
+        <v>2595</v>
       </c>
       <c r="X18" s="2">
-        <v>24</v>
+        <v>999</v>
       </c>
       <c r="Y18" s="2">
-        <v>50942.5</v>
+        <v>50167.957030999998</v>
       </c>
       <c r="Z18" s="2">
-        <v>4.7100000000000001E-4</v>
+        <v>1.9913E-2</v>
       </c>
     </row>
     <row r="19" spans="5:26" x14ac:dyDescent="0.2">
@@ -2166,19 +2120,19 @@
         <v>1000</v>
       </c>
       <c r="K19" s="2">
-        <v>36434</v>
+        <v>2876</v>
       </c>
       <c r="L19" s="2">
-        <v>8994</v>
+        <v>2597</v>
       </c>
       <c r="M19" s="2">
-        <v>31</v>
+        <v>999</v>
       </c>
       <c r="N19" s="2">
-        <v>50276.601562000003</v>
+        <v>49978.101562000003</v>
       </c>
       <c r="O19" s="2">
-        <v>6.1700000000000004E-4</v>
+        <v>1.9989E-2</v>
       </c>
       <c r="P19" s="2">
         <v>2</v>
@@ -2199,19 +2153,19 @@
         <v>1000</v>
       </c>
       <c r="V19" s="2">
-        <v>40220</v>
+        <v>3729</v>
       </c>
       <c r="W19" s="2">
-        <v>9137</v>
+        <v>2997</v>
       </c>
       <c r="X19" s="2">
-        <v>34</v>
+        <v>999</v>
       </c>
       <c r="Y19" s="2">
-        <v>50569.648437999997</v>
+        <v>49798.925780999998</v>
       </c>
       <c r="Z19" s="2">
-        <v>6.7199999999999996E-4</v>
+        <v>2.0060999999999999E-2</v>
       </c>
     </row>
     <row r="20" spans="5:26" x14ac:dyDescent="0.2">
@@ -2234,19 +2188,19 @@
         <v>1000</v>
       </c>
       <c r="K20" s="2">
-        <v>36663</v>
+        <v>2591</v>
       </c>
       <c r="L20" s="2">
-        <v>9065</v>
+        <v>2320</v>
       </c>
       <c r="M20" s="2">
-        <v>28</v>
+        <v>997</v>
       </c>
       <c r="N20" s="2">
-        <v>49990.132812000003</v>
+        <v>47702.074219000002</v>
       </c>
       <c r="O20" s="2">
-        <v>5.5999999999999995E-4</v>
+        <v>2.0900999999999999E-2</v>
       </c>
       <c r="P20" s="2">
         <v>3</v>
@@ -2267,19 +2221,19 @@
         <v>1000</v>
       </c>
       <c r="V20" s="2">
-        <v>31007</v>
+        <v>3564</v>
       </c>
       <c r="W20" s="2">
-        <v>9314</v>
+        <v>2848</v>
       </c>
       <c r="X20" s="2">
-        <v>28</v>
+        <v>996</v>
       </c>
       <c r="Y20" s="2">
-        <v>51429.449219000002</v>
+        <v>50231.199219000002</v>
       </c>
       <c r="Z20" s="2">
-        <v>5.44E-4</v>
+        <v>1.9827999999999998E-2</v>
       </c>
     </row>
     <row r="21" spans="5:26" x14ac:dyDescent="0.2">
@@ -2302,19 +2256,19 @@
         <v>1000</v>
       </c>
       <c r="K21" s="2">
-        <v>27927</v>
+        <v>2858</v>
       </c>
       <c r="L21" s="2">
-        <v>9304</v>
+        <v>2586</v>
       </c>
       <c r="M21" s="2">
-        <v>30</v>
+        <v>999</v>
       </c>
       <c r="N21" s="2">
-        <v>51344.898437999997</v>
+        <v>49329.3125</v>
       </c>
       <c r="O21" s="2">
-        <v>5.8399999999999999E-4</v>
+        <v>2.0251999999999999E-2</v>
       </c>
       <c r="P21" s="2">
         <v>4</v>
@@ -2335,19 +2289,19 @@
         <v>1000</v>
       </c>
       <c r="V21" s="2">
-        <v>36350</v>
+        <v>14151</v>
       </c>
       <c r="W21" s="2">
-        <v>8997</v>
+        <v>7453</v>
       </c>
       <c r="X21" s="2">
-        <v>30</v>
+        <v>342</v>
       </c>
       <c r="Y21" s="2">
-        <v>49807.757812000003</v>
+        <v>49339.851562000003</v>
       </c>
       <c r="Z21" s="2">
-        <v>6.02E-4</v>
+        <v>6.9319999999999998E-3</v>
       </c>
     </row>
     <row r="22" spans="5:26" x14ac:dyDescent="0.2">
@@ -2370,19 +2324,19 @@
         <v>1000</v>
       </c>
       <c r="K22" s="2">
-        <v>30361</v>
+        <v>2744</v>
       </c>
       <c r="L22" s="2">
-        <v>9053</v>
+        <v>2468</v>
       </c>
       <c r="M22" s="2">
-        <v>33</v>
+        <v>999</v>
       </c>
       <c r="N22" s="2">
-        <v>49959.527344000002</v>
+        <v>51574.144530999998</v>
       </c>
       <c r="O22" s="2">
-        <v>6.6100000000000002E-4</v>
+        <v>1.9369999999999998E-2</v>
       </c>
       <c r="P22" s="2">
         <v>5</v>
@@ -2403,19 +2357,19 @@
         <v>1000</v>
       </c>
       <c r="V22" s="2">
-        <v>32946</v>
+        <v>3784</v>
       </c>
       <c r="W22" s="2">
-        <v>8909</v>
+        <v>3017</v>
       </c>
       <c r="X22" s="2">
-        <v>33</v>
+        <v>998</v>
       </c>
       <c r="Y22" s="2">
-        <v>49529.917969000002</v>
+        <v>51545.464844000002</v>
       </c>
       <c r="Z22" s="2">
-        <v>6.6600000000000003E-4</v>
+        <v>1.9362000000000001E-2</v>
       </c>
     </row>
     <row r="23" spans="5:26" x14ac:dyDescent="0.2">
@@ -2438,19 +2392,19 @@
         <v>1000</v>
       </c>
       <c r="K23" s="2">
-        <v>33430</v>
+        <v>2765</v>
       </c>
       <c r="L23" s="2">
-        <v>9061</v>
+        <v>2487</v>
       </c>
       <c r="M23" s="2">
-        <v>25</v>
+        <v>999</v>
       </c>
       <c r="N23" s="2">
-        <v>50264.347655999998</v>
+        <v>49147.855469000002</v>
       </c>
       <c r="O23" s="2">
-        <v>4.9700000000000005E-4</v>
+        <v>2.0326E-2</v>
       </c>
       <c r="P23" s="2">
         <v>6</v>
@@ -2471,19 +2425,19 @@
         <v>1000</v>
       </c>
       <c r="V23" s="2">
-        <v>39095</v>
+        <v>3594</v>
       </c>
       <c r="W23" s="2">
-        <v>8880</v>
+        <v>2912</v>
       </c>
       <c r="X23" s="2">
-        <v>18</v>
+        <v>906</v>
       </c>
       <c r="Y23" s="2">
-        <v>49554.851562000003</v>
+        <v>50389.492187999997</v>
       </c>
       <c r="Z23" s="2">
-        <v>3.6299999999999999E-4</v>
+        <v>1.7979999999999999E-2</v>
       </c>
     </row>
     <row r="24" spans="5:26" x14ac:dyDescent="0.2">
@@ -2506,19 +2460,19 @@
         <v>1000</v>
       </c>
       <c r="K24" s="2">
-        <v>34987</v>
+        <v>2755</v>
       </c>
       <c r="L24" s="2">
-        <v>8744</v>
+        <v>2488</v>
       </c>
       <c r="M24" s="2">
-        <v>27</v>
+        <v>999</v>
       </c>
       <c r="N24" s="2">
-        <v>48263.660155999998</v>
+        <v>50448.085937999997</v>
       </c>
       <c r="O24" s="2">
-        <v>5.5900000000000004E-4</v>
+        <v>1.9803000000000001E-2</v>
       </c>
       <c r="P24" s="2">
         <v>7</v>
@@ -2539,19 +2493,19 @@
         <v>1000</v>
       </c>
       <c r="V24" s="2">
-        <v>36617</v>
+        <v>3803</v>
       </c>
       <c r="W24" s="2">
-        <v>9030</v>
+        <v>3051</v>
       </c>
       <c r="X24" s="2">
-        <v>30</v>
+        <v>999</v>
       </c>
       <c r="Y24" s="2">
-        <v>49882.375</v>
+        <v>50255.117187999997</v>
       </c>
       <c r="Z24" s="2">
-        <v>6.0099999999999997E-4</v>
+        <v>1.9879000000000001E-2</v>
       </c>
     </row>
     <row r="25" spans="5:26" x14ac:dyDescent="0.2">
@@ -2574,19 +2528,19 @@
         <v>1000</v>
       </c>
       <c r="K25" s="2">
-        <v>30302</v>
+        <v>2681</v>
       </c>
       <c r="L25" s="2">
-        <v>9013</v>
+        <v>2386</v>
       </c>
       <c r="M25" s="2">
-        <v>36</v>
+        <v>998</v>
       </c>
       <c r="N25" s="2">
-        <v>50618.886719000002</v>
+        <v>51008.28125</v>
       </c>
       <c r="O25" s="2">
-        <v>7.1100000000000004E-4</v>
+        <v>1.9564999999999999E-2</v>
       </c>
       <c r="P25" s="2">
         <v>8</v>
@@ -2607,19 +2561,19 @@
         <v>1000</v>
       </c>
       <c r="V25" s="2">
-        <v>32445</v>
+        <v>3730</v>
       </c>
       <c r="W25" s="2">
-        <v>8750</v>
+        <v>3009</v>
       </c>
       <c r="X25" s="2">
-        <v>30</v>
+        <v>997</v>
       </c>
       <c r="Y25" s="2">
-        <v>48959.371094000002</v>
+        <v>48498.894530999998</v>
       </c>
       <c r="Z25" s="2">
-        <v>6.1300000000000005E-4</v>
+        <v>2.0556999999999999E-2</v>
       </c>
     </row>
     <row r="26" spans="5:26" x14ac:dyDescent="0.2">
@@ -2642,53 +2596,31 @@
         <v>1000</v>
       </c>
       <c r="K26" s="2">
-        <v>28968</v>
+        <v>2868</v>
       </c>
       <c r="L26" s="2">
-        <v>8723</v>
+        <v>2549</v>
       </c>
       <c r="M26" s="2">
-        <v>29</v>
+        <v>999</v>
       </c>
       <c r="N26" s="2">
-        <v>48159.304687999997</v>
+        <v>51017.875</v>
       </c>
       <c r="O26" s="2">
-        <v>6.02E-4</v>
-      </c>
-      <c r="P26" s="2">
-        <v>9</v>
-      </c>
-      <c r="Q26" s="2">
-        <v>1000</v>
-      </c>
-      <c r="R26" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="S26" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="T26" s="2">
-        <v>50</v>
-      </c>
-      <c r="U26" s="2">
-        <v>1000</v>
-      </c>
-      <c r="V26" s="2">
-        <v>58443</v>
-      </c>
-      <c r="W26" s="2">
-        <v>8982</v>
-      </c>
-      <c r="X26" s="2">
-        <v>20</v>
-      </c>
-      <c r="Y26" s="2">
-        <v>49613.976562000003</v>
-      </c>
-      <c r="Z26" s="2">
-        <v>4.0299999999999998E-4</v>
-      </c>
+        <v>1.9581000000000001E-2</v>
+      </c>
+      <c r="P26" s="2"/>
+      <c r="Q26" s="2"/>
+      <c r="R26" s="2"/>
+      <c r="S26" s="2"/>
+      <c r="T26" s="2"/>
+      <c r="U26" s="2"/>
+      <c r="V26" s="2"/>
+      <c r="W26" s="2"/>
+      <c r="X26" s="2"/>
+      <c r="Y26" s="2"/>
+      <c r="Z26" s="2"/>
     </row>
     <row r="27" spans="5:26" x14ac:dyDescent="0.2">
       <c r="E27" s="2">
@@ -2710,53 +2642,31 @@
         <v>1000</v>
       </c>
       <c r="K27" s="2">
-        <v>34286</v>
+        <v>2649</v>
       </c>
       <c r="L27" s="2">
-        <v>9181</v>
+        <v>2388</v>
       </c>
       <c r="M27" s="2">
-        <v>37</v>
+        <v>998</v>
       </c>
       <c r="N27" s="2">
-        <v>51157.714844000002</v>
+        <v>51240.632812000003</v>
       </c>
       <c r="O27" s="2">
-        <v>7.2300000000000001E-4</v>
-      </c>
-      <c r="P27" s="2">
-        <v>10</v>
-      </c>
-      <c r="Q27" s="2">
-        <v>1000</v>
-      </c>
-      <c r="R27" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="S27" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="T27" s="2">
-        <v>50</v>
-      </c>
-      <c r="U27" s="2">
-        <v>1000</v>
-      </c>
-      <c r="V27" s="2">
-        <v>42689</v>
-      </c>
-      <c r="W27" s="2">
-        <v>8910</v>
-      </c>
-      <c r="X27" s="2">
-        <v>25</v>
-      </c>
-      <c r="Y27" s="2">
-        <v>49720.515625</v>
-      </c>
-      <c r="Z27" s="2">
-        <v>5.0299999999999997E-4</v>
-      </c>
+        <v>1.9477000000000001E-2</v>
+      </c>
+      <c r="P27" s="2"/>
+      <c r="Q27" s="2"/>
+      <c r="R27" s="2"/>
+      <c r="S27" s="2"/>
+      <c r="T27" s="2"/>
+      <c r="U27" s="2"/>
+      <c r="V27" s="2"/>
+      <c r="W27" s="2"/>
+      <c r="X27" s="2"/>
+      <c r="Y27" s="2"/>
+      <c r="Z27" s="2"/>
     </row>
     <row r="28" spans="5:26" x14ac:dyDescent="0.2">
       <c r="E28" s="3" t="s">
@@ -2784,23 +2694,23 @@
       </c>
       <c r="K28" s="2">
         <f>AVERAGE(K18:K27)</f>
-        <v>33613.1</v>
+        <v>2756</v>
       </c>
       <c r="L28" s="2">
         <f t="shared" si="2"/>
-        <v>9017.6</v>
+        <v>2475.3000000000002</v>
       </c>
       <c r="M28" s="2">
         <f t="shared" si="2"/>
-        <v>29.9</v>
+        <v>998.4</v>
       </c>
       <c r="N28" s="2">
         <f t="shared" si="2"/>
-        <v>49983.373828099997</v>
+        <v>50142.787890599997</v>
       </c>
       <c r="O28" s="2">
         <f t="shared" si="2"/>
-        <v>5.976E-4</v>
+        <v>1.9921100000000001E-2</v>
       </c>
       <c r="P28" s="3" t="s">
         <v>14</v>
@@ -2827,23 +2737,23 @@
       </c>
       <c r="V28" s="2">
         <f t="shared" si="3"/>
-        <v>38381</v>
+        <v>4945.375</v>
       </c>
       <c r="W28" s="2">
         <f t="shared" si="3"/>
-        <v>9014.1</v>
+        <v>3485.25</v>
       </c>
       <c r="X28" s="2">
         <f t="shared" si="3"/>
-        <v>27.2</v>
+        <v>904.5</v>
       </c>
       <c r="Y28" s="2">
         <f t="shared" si="3"/>
-        <v>50001.036328100003</v>
+        <v>50028.362793</v>
       </c>
       <c r="Z28" s="2">
         <f t="shared" si="3"/>
-        <v>5.4379999999999988E-4</v>
+        <v>1.8063999999999997E-2</v>
       </c>
     </row>
     <row r="29" spans="5:26" x14ac:dyDescent="0.2">
@@ -4655,839 +4565,355 @@
       <c r="Z57" s="16"/>
     </row>
     <row r="58" spans="5:26" x14ac:dyDescent="0.2">
-      <c r="E58" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="F58" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="G58" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="H58" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="I58" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="J58" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="K58" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="L58" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="M58" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="N58" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="O58" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="P58" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q58" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="R58" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="S58" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="T58" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="U58" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="V58" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="W58" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="X58" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="Y58" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="Z58" s="6" t="s">
-        <v>10</v>
-      </c>
+      <c r="E58" s="2"/>
+      <c r="F58" s="2"/>
+      <c r="G58" s="2"/>
+      <c r="H58" s="2"/>
+      <c r="I58" s="2"/>
+      <c r="J58" s="2"/>
+      <c r="K58" s="2"/>
+      <c r="L58" s="2"/>
+      <c r="M58" s="2"/>
+      <c r="N58" s="2"/>
+      <c r="O58" s="2"/>
+      <c r="P58" s="5"/>
+      <c r="Q58" s="6"/>
+      <c r="R58" s="6"/>
+      <c r="S58" s="6"/>
+      <c r="T58" s="6"/>
+      <c r="U58" s="6"/>
+      <c r="V58" s="6"/>
+      <c r="W58" s="6"/>
+      <c r="X58" s="6"/>
+      <c r="Y58" s="6"/>
+      <c r="Z58" s="6"/>
     </row>
     <row r="59" spans="5:26" x14ac:dyDescent="0.2">
-      <c r="E59" s="2">
-        <v>1</v>
-      </c>
-      <c r="F59" s="2">
-        <v>1000</v>
-      </c>
-      <c r="G59" s="2">
-        <v>0.4</v>
-      </c>
-      <c r="H59" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="I59" s="2">
-        <v>50</v>
-      </c>
-      <c r="J59" s="2">
-        <v>1000</v>
-      </c>
-      <c r="K59" s="2">
-        <v>43057</v>
-      </c>
-      <c r="L59" s="2">
-        <v>9076</v>
-      </c>
-      <c r="M59" s="2">
-        <v>26</v>
-      </c>
-      <c r="N59" s="2">
-        <v>49953.101562000003</v>
-      </c>
-      <c r="O59" s="2">
-        <v>5.1999999999999995E-4</v>
-      </c>
-      <c r="P59" s="5">
-        <v>1</v>
-      </c>
-      <c r="Q59" s="6">
-        <v>1000</v>
-      </c>
-      <c r="R59" s="6">
-        <v>0.6</v>
-      </c>
-      <c r="S59" s="6">
-        <v>0.2</v>
-      </c>
-      <c r="T59" s="6">
-        <v>50</v>
-      </c>
-      <c r="U59" s="6">
-        <v>1000</v>
-      </c>
-      <c r="V59" s="6">
-        <v>62216</v>
-      </c>
-      <c r="W59" s="6">
-        <v>9040</v>
-      </c>
-      <c r="X59" s="6">
-        <v>20</v>
-      </c>
-      <c r="Y59" s="6">
-        <v>50082.671875</v>
-      </c>
-      <c r="Z59" s="6">
-        <v>3.9899999999999999E-4</v>
-      </c>
+      <c r="E59" s="2"/>
+      <c r="F59" s="2"/>
+      <c r="G59" s="2"/>
+      <c r="H59" s="2"/>
+      <c r="I59" s="2"/>
+      <c r="J59" s="2"/>
+      <c r="K59" s="2"/>
+      <c r="L59" s="2"/>
+      <c r="M59" s="2"/>
+      <c r="N59" s="2"/>
+      <c r="O59" s="2"/>
+      <c r="P59" s="5"/>
+      <c r="Q59" s="6"/>
+      <c r="R59" s="6"/>
+      <c r="S59" s="6"/>
+      <c r="T59" s="6"/>
+      <c r="U59" s="6"/>
+      <c r="V59" s="6"/>
+      <c r="W59" s="6"/>
+      <c r="X59" s="6"/>
+      <c r="Y59" s="6"/>
+      <c r="Z59" s="6"/>
     </row>
     <row r="60" spans="5:26" x14ac:dyDescent="0.2">
-      <c r="E60" s="2">
-        <v>2</v>
-      </c>
-      <c r="F60" s="2">
-        <v>1000</v>
-      </c>
-      <c r="G60" s="2">
-        <v>0.4</v>
-      </c>
-      <c r="H60" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="I60" s="2">
-        <v>50</v>
-      </c>
-      <c r="J60" s="2">
-        <v>1000</v>
-      </c>
-      <c r="K60" s="2">
-        <v>49485</v>
-      </c>
-      <c r="L60" s="2">
-        <v>8960</v>
-      </c>
-      <c r="M60" s="2">
-        <v>29</v>
-      </c>
-      <c r="N60" s="2">
-        <v>49606.871094000002</v>
-      </c>
-      <c r="O60" s="2">
-        <v>5.8500000000000002E-4</v>
-      </c>
-      <c r="P60" s="5">
-        <v>2</v>
-      </c>
-      <c r="Q60" s="6">
-        <v>1000</v>
-      </c>
-      <c r="R60" s="6">
-        <v>0.6</v>
-      </c>
-      <c r="S60" s="6">
-        <v>0.2</v>
-      </c>
-      <c r="T60" s="6">
-        <v>50</v>
-      </c>
-      <c r="U60" s="6">
-        <v>1000</v>
-      </c>
-      <c r="V60" s="6">
-        <v>62408</v>
-      </c>
-      <c r="W60" s="6">
-        <v>9056</v>
-      </c>
-      <c r="X60" s="6">
-        <v>27</v>
-      </c>
-      <c r="Y60" s="6">
-        <v>49893.308594000002</v>
-      </c>
-      <c r="Z60" s="6">
-        <v>5.4100000000000003E-4</v>
-      </c>
+      <c r="E60" s="2"/>
+      <c r="F60" s="2"/>
+      <c r="G60" s="2"/>
+      <c r="H60" s="2"/>
+      <c r="I60" s="2"/>
+      <c r="J60" s="2"/>
+      <c r="K60" s="2"/>
+      <c r="L60" s="2"/>
+      <c r="M60" s="2"/>
+      <c r="N60" s="2"/>
+      <c r="O60" s="2"/>
+      <c r="P60" s="5"/>
+      <c r="Q60" s="6"/>
+      <c r="R60" s="6"/>
+      <c r="S60" s="6"/>
+      <c r="T60" s="6"/>
+      <c r="U60" s="6"/>
+      <c r="V60" s="6"/>
+      <c r="W60" s="6"/>
+      <c r="X60" s="6"/>
+      <c r="Y60" s="6"/>
+      <c r="Z60" s="6"/>
     </row>
     <row r="61" spans="5:26" x14ac:dyDescent="0.2">
-      <c r="E61" s="2">
-        <v>3</v>
-      </c>
-      <c r="F61" s="2">
-        <v>1000</v>
-      </c>
-      <c r="G61" s="2">
-        <v>0.4</v>
-      </c>
-      <c r="H61" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="I61" s="2">
-        <v>50</v>
-      </c>
-      <c r="J61" s="2">
-        <v>1000</v>
-      </c>
-      <c r="K61" s="2">
-        <v>51151</v>
-      </c>
-      <c r="L61" s="2">
-        <v>8787</v>
-      </c>
-      <c r="M61" s="2">
-        <v>11</v>
-      </c>
-      <c r="N61" s="2">
-        <v>48529.035155999998</v>
-      </c>
-      <c r="O61" s="2">
-        <v>2.2699999999999999E-4</v>
-      </c>
-      <c r="P61" s="5">
-        <v>3</v>
-      </c>
-      <c r="Q61" s="6">
-        <v>1000</v>
-      </c>
-      <c r="R61" s="6">
-        <v>0.6</v>
-      </c>
-      <c r="S61" s="6">
-        <v>0.2</v>
-      </c>
-      <c r="T61" s="6">
-        <v>50</v>
-      </c>
-      <c r="U61" s="6">
-        <v>1000</v>
-      </c>
-      <c r="V61" s="6">
-        <v>32687</v>
-      </c>
-      <c r="W61" s="6">
-        <v>8968</v>
-      </c>
-      <c r="X61" s="6">
-        <v>10</v>
-      </c>
-      <c r="Y61" s="6">
-        <v>49334.574219000002</v>
-      </c>
-      <c r="Z61" s="6">
-        <v>2.03E-4</v>
-      </c>
+      <c r="E61" s="2"/>
+      <c r="F61" s="2"/>
+      <c r="G61" s="2"/>
+      <c r="H61" s="2"/>
+      <c r="I61" s="2"/>
+      <c r="J61" s="2"/>
+      <c r="K61" s="2"/>
+      <c r="L61" s="2"/>
+      <c r="M61" s="2"/>
+      <c r="N61" s="2"/>
+      <c r="O61" s="2"/>
+      <c r="P61" s="5"/>
+      <c r="Q61" s="6"/>
+      <c r="R61" s="6"/>
+      <c r="S61" s="6"/>
+      <c r="T61" s="6"/>
+      <c r="U61" s="6"/>
+      <c r="V61" s="6"/>
+      <c r="W61" s="6"/>
+      <c r="X61" s="6"/>
+      <c r="Y61" s="6"/>
+      <c r="Z61" s="6"/>
     </row>
     <row r="62" spans="5:26" x14ac:dyDescent="0.2">
-      <c r="E62" s="2">
-        <v>4</v>
-      </c>
-      <c r="F62" s="2">
-        <v>1000</v>
-      </c>
-      <c r="G62" s="2">
-        <v>0.4</v>
-      </c>
-      <c r="H62" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="I62" s="2">
-        <v>50</v>
-      </c>
-      <c r="J62" s="2">
-        <v>1000</v>
-      </c>
-      <c r="K62" s="2">
-        <v>49356</v>
-      </c>
-      <c r="L62" s="2">
-        <v>8993</v>
-      </c>
-      <c r="M62" s="2">
-        <v>18</v>
-      </c>
-      <c r="N62" s="2">
-        <v>49991.894530999998</v>
-      </c>
-      <c r="O62" s="2">
-        <v>3.6000000000000002E-4</v>
-      </c>
-      <c r="P62" s="5">
-        <v>4</v>
-      </c>
-      <c r="Q62" s="6">
-        <v>1000</v>
-      </c>
-      <c r="R62" s="6">
-        <v>0.6</v>
-      </c>
-      <c r="S62" s="6">
-        <v>0.2</v>
-      </c>
-      <c r="T62" s="6">
-        <v>50</v>
-      </c>
-      <c r="U62" s="6">
-        <v>1000</v>
-      </c>
-      <c r="V62" s="6">
-        <v>45959</v>
-      </c>
-      <c r="W62" s="6">
-        <v>9034</v>
-      </c>
-      <c r="X62" s="6">
-        <v>19</v>
-      </c>
-      <c r="Y62" s="6">
-        <v>49756.675780999998</v>
-      </c>
-      <c r="Z62" s="6">
-        <v>3.8200000000000002E-4</v>
-      </c>
+      <c r="E62" s="2"/>
+      <c r="F62" s="2"/>
+      <c r="G62" s="2"/>
+      <c r="H62" s="2"/>
+      <c r="I62" s="2"/>
+      <c r="J62" s="2"/>
+      <c r="K62" s="2"/>
+      <c r="L62" s="2"/>
+      <c r="M62" s="2"/>
+      <c r="N62" s="2"/>
+      <c r="O62" s="2"/>
+      <c r="P62" s="5"/>
+      <c r="Q62" s="6"/>
+      <c r="R62" s="6"/>
+      <c r="S62" s="6"/>
+      <c r="T62" s="6"/>
+      <c r="U62" s="6"/>
+      <c r="V62" s="6"/>
+      <c r="W62" s="6"/>
+      <c r="X62" s="6"/>
+      <c r="Y62" s="6"/>
+      <c r="Z62" s="6"/>
     </row>
     <row r="63" spans="5:26" x14ac:dyDescent="0.2">
-      <c r="E63" s="2">
-        <v>5</v>
-      </c>
-      <c r="F63" s="2">
-        <v>1000</v>
-      </c>
-      <c r="G63" s="2">
-        <v>0.4</v>
-      </c>
-      <c r="H63" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="I63" s="2">
-        <v>50</v>
-      </c>
-      <c r="J63" s="2">
-        <v>1000</v>
-      </c>
-      <c r="K63" s="2">
-        <v>50794</v>
-      </c>
-      <c r="L63" s="2">
-        <v>9288</v>
-      </c>
-      <c r="M63" s="2">
-        <v>28</v>
-      </c>
-      <c r="N63" s="2">
-        <v>51322.902344000002</v>
-      </c>
-      <c r="O63" s="2">
-        <v>5.4600000000000004E-4</v>
-      </c>
-      <c r="P63" s="5">
-        <v>5</v>
-      </c>
-      <c r="Q63" s="6">
-        <v>1000</v>
-      </c>
-      <c r="R63" s="6">
-        <v>0.6</v>
-      </c>
-      <c r="S63" s="6">
-        <v>0.2</v>
-      </c>
-      <c r="T63" s="6">
-        <v>50</v>
-      </c>
-      <c r="U63" s="6">
-        <v>1000</v>
-      </c>
-      <c r="V63" s="6">
-        <v>56579</v>
-      </c>
-      <c r="W63" s="6">
-        <v>9123</v>
-      </c>
-      <c r="X63" s="6">
-        <v>36</v>
-      </c>
-      <c r="Y63" s="6">
-        <v>50635.746094000002</v>
-      </c>
-      <c r="Z63" s="6">
-        <v>7.1100000000000004E-4</v>
-      </c>
+      <c r="E63" s="2"/>
+      <c r="F63" s="2"/>
+      <c r="G63" s="2"/>
+      <c r="H63" s="2"/>
+      <c r="I63" s="2"/>
+      <c r="J63" s="2"/>
+      <c r="K63" s="2"/>
+      <c r="L63" s="2"/>
+      <c r="M63" s="2"/>
+      <c r="N63" s="2"/>
+      <c r="O63" s="2"/>
+      <c r="P63" s="5"/>
+      <c r="Q63" s="6"/>
+      <c r="R63" s="6"/>
+      <c r="S63" s="6"/>
+      <c r="T63" s="6"/>
+      <c r="U63" s="6"/>
+      <c r="V63" s="6"/>
+      <c r="W63" s="6"/>
+      <c r="X63" s="6"/>
+      <c r="Y63" s="6"/>
+      <c r="Z63" s="6"/>
     </row>
     <row r="64" spans="5:26" x14ac:dyDescent="0.2">
-      <c r="E64" s="2">
-        <v>6</v>
-      </c>
-      <c r="F64" s="2">
-        <v>1000</v>
-      </c>
-      <c r="G64" s="2">
-        <v>0.4</v>
-      </c>
-      <c r="H64" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="I64" s="2">
-        <v>50</v>
-      </c>
-      <c r="J64" s="2">
-        <v>1000</v>
-      </c>
-      <c r="K64" s="2">
-        <v>43398</v>
-      </c>
-      <c r="L64" s="2">
-        <v>9117</v>
-      </c>
-      <c r="M64" s="2">
-        <v>26</v>
-      </c>
-      <c r="N64" s="2">
-        <v>50227.761719000002</v>
-      </c>
-      <c r="O64" s="2">
-        <v>5.1800000000000001E-4</v>
-      </c>
-      <c r="P64" s="5">
-        <v>6</v>
-      </c>
-      <c r="Q64" s="6">
-        <v>1000</v>
-      </c>
-      <c r="R64" s="6">
-        <v>0.6</v>
-      </c>
-      <c r="S64" s="6">
-        <v>0.2</v>
-      </c>
-      <c r="T64" s="6">
-        <v>50</v>
-      </c>
-      <c r="U64" s="6">
-        <v>1000</v>
-      </c>
-      <c r="V64" s="6">
-        <v>57287</v>
-      </c>
-      <c r="W64" s="6">
-        <v>8725</v>
-      </c>
-      <c r="X64" s="6">
-        <v>30</v>
-      </c>
-      <c r="Y64" s="6">
-        <v>48244.898437999997</v>
-      </c>
-      <c r="Z64" s="6">
-        <v>6.2200000000000005E-4</v>
-      </c>
+      <c r="E64" s="2"/>
+      <c r="F64" s="2"/>
+      <c r="G64" s="2"/>
+      <c r="H64" s="2"/>
+      <c r="I64" s="2"/>
+      <c r="J64" s="2"/>
+      <c r="K64" s="2"/>
+      <c r="L64" s="2"/>
+      <c r="M64" s="2"/>
+      <c r="N64" s="2"/>
+      <c r="O64" s="2"/>
+      <c r="P64" s="5"/>
+      <c r="Q64" s="6"/>
+      <c r="R64" s="6"/>
+      <c r="S64" s="6"/>
+      <c r="T64" s="6"/>
+      <c r="U64" s="6"/>
+      <c r="V64" s="6"/>
+      <c r="W64" s="6"/>
+      <c r="X64" s="6"/>
+      <c r="Y64" s="6"/>
+      <c r="Z64" s="6"/>
     </row>
     <row r="65" spans="5:26" x14ac:dyDescent="0.2">
-      <c r="E65" s="2">
-        <v>7</v>
-      </c>
-      <c r="F65" s="2">
-        <v>1000</v>
-      </c>
-      <c r="G65" s="2">
-        <v>0.4</v>
-      </c>
-      <c r="H65" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="I65" s="2">
-        <v>50</v>
-      </c>
-      <c r="J65" s="2">
-        <v>1000</v>
-      </c>
-      <c r="K65" s="2">
-        <v>43285</v>
-      </c>
-      <c r="L65" s="2">
-        <v>9231</v>
-      </c>
-      <c r="M65" s="2">
-        <v>26</v>
-      </c>
-      <c r="N65" s="2">
-        <v>50713.605469000002</v>
-      </c>
-      <c r="O65" s="2">
-        <v>5.13E-4</v>
-      </c>
-      <c r="P65" s="5">
-        <v>7</v>
-      </c>
-      <c r="Q65" s="6">
-        <v>1000</v>
-      </c>
-      <c r="R65" s="6">
-        <v>0.6</v>
-      </c>
-      <c r="S65" s="6">
-        <v>0.2</v>
-      </c>
-      <c r="T65" s="6">
-        <v>50</v>
-      </c>
-      <c r="U65" s="6">
-        <v>1000</v>
-      </c>
-      <c r="V65" s="6">
-        <v>63088</v>
-      </c>
-      <c r="W65" s="6">
-        <v>9209</v>
-      </c>
-      <c r="X65" s="6">
-        <v>32</v>
-      </c>
-      <c r="Y65" s="6">
-        <v>50476.210937999997</v>
-      </c>
-      <c r="Z65" s="6">
-        <v>6.3400000000000001E-4</v>
-      </c>
+      <c r="E65" s="2"/>
+      <c r="F65" s="2"/>
+      <c r="G65" s="2"/>
+      <c r="H65" s="2"/>
+      <c r="I65" s="2"/>
+      <c r="J65" s="2"/>
+      <c r="K65" s="2"/>
+      <c r="L65" s="2"/>
+      <c r="M65" s="2"/>
+      <c r="N65" s="2"/>
+      <c r="O65" s="2"/>
+      <c r="P65" s="5"/>
+      <c r="Q65" s="6"/>
+      <c r="R65" s="6"/>
+      <c r="S65" s="6"/>
+      <c r="T65" s="6"/>
+      <c r="U65" s="6"/>
+      <c r="V65" s="6"/>
+      <c r="W65" s="6"/>
+      <c r="X65" s="6"/>
+      <c r="Y65" s="6"/>
+      <c r="Z65" s="6"/>
     </row>
     <row r="66" spans="5:26" x14ac:dyDescent="0.2">
-      <c r="E66" s="2">
-        <v>8</v>
-      </c>
-      <c r="F66" s="2">
-        <v>1000</v>
-      </c>
-      <c r="G66" s="2">
-        <v>0.4</v>
-      </c>
-      <c r="H66" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="I66" s="2">
-        <v>50</v>
-      </c>
-      <c r="J66" s="2">
-        <v>1000</v>
-      </c>
-      <c r="K66" s="2">
-        <v>42296</v>
-      </c>
-      <c r="L66" s="2">
-        <v>8780</v>
-      </c>
-      <c r="M66" s="2">
-        <v>28</v>
-      </c>
-      <c r="N66" s="2">
-        <v>49008.507812000003</v>
-      </c>
-      <c r="O66" s="2">
-        <v>5.71E-4</v>
-      </c>
-      <c r="P66" s="5">
-        <v>8</v>
-      </c>
-      <c r="Q66" s="6">
-        <v>1000</v>
-      </c>
-      <c r="R66" s="6">
-        <v>0.6</v>
-      </c>
-      <c r="S66" s="6">
-        <v>0.2</v>
-      </c>
-      <c r="T66" s="6">
-        <v>50</v>
-      </c>
-      <c r="U66" s="6">
-        <v>1000</v>
-      </c>
-      <c r="V66" s="6">
-        <v>54507</v>
-      </c>
-      <c r="W66" s="6">
-        <v>8692</v>
-      </c>
-      <c r="X66" s="6">
-        <v>30</v>
-      </c>
-      <c r="Y66" s="6">
-        <v>48517.589844000002</v>
-      </c>
-      <c r="Z66" s="6">
-        <v>6.1799999999999995E-4</v>
-      </c>
+      <c r="E66" s="2"/>
+      <c r="F66" s="2"/>
+      <c r="G66" s="2"/>
+      <c r="H66" s="2"/>
+      <c r="I66" s="2"/>
+      <c r="J66" s="2"/>
+      <c r="K66" s="2"/>
+      <c r="L66" s="2"/>
+      <c r="M66" s="2"/>
+      <c r="N66" s="2"/>
+      <c r="O66" s="2"/>
+      <c r="P66" s="5"/>
+      <c r="Q66" s="6"/>
+      <c r="R66" s="6"/>
+      <c r="S66" s="6"/>
+      <c r="T66" s="6"/>
+      <c r="U66" s="6"/>
+      <c r="V66" s="6"/>
+      <c r="W66" s="6"/>
+      <c r="X66" s="6"/>
+      <c r="Y66" s="6"/>
+      <c r="Z66" s="6"/>
     </row>
     <row r="67" spans="5:26" x14ac:dyDescent="0.2">
-      <c r="E67" s="2">
-        <v>9</v>
-      </c>
-      <c r="F67" s="2">
-        <v>1000</v>
-      </c>
-      <c r="G67" s="2">
-        <v>0.4</v>
-      </c>
-      <c r="H67" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="I67" s="2">
-        <v>50</v>
-      </c>
-      <c r="J67" s="2">
-        <v>1000</v>
-      </c>
-      <c r="K67" s="2">
-        <v>52432</v>
-      </c>
-      <c r="L67" s="2">
-        <v>8990</v>
-      </c>
-      <c r="M67" s="2">
-        <v>26</v>
-      </c>
-      <c r="N67" s="2">
-        <v>49652.65625</v>
-      </c>
-      <c r="O67" s="2">
-        <v>5.2400000000000005E-4</v>
-      </c>
-      <c r="P67" s="5">
-        <v>9</v>
-      </c>
-      <c r="Q67" s="6">
-        <v>1000</v>
-      </c>
-      <c r="R67" s="6">
-        <v>0.6</v>
-      </c>
-      <c r="S67" s="6">
-        <v>0.2</v>
-      </c>
-      <c r="T67" s="6">
-        <v>50</v>
-      </c>
-      <c r="U67" s="6">
-        <v>1000</v>
-      </c>
-      <c r="V67" s="6">
-        <v>34235</v>
-      </c>
-      <c r="W67" s="6">
-        <v>9430</v>
-      </c>
-      <c r="X67" s="6">
-        <v>10</v>
-      </c>
-      <c r="Y67" s="6">
-        <v>51637.292969000002</v>
-      </c>
-      <c r="Z67" s="6">
-        <v>1.94E-4</v>
-      </c>
+      <c r="E67" s="2"/>
+      <c r="F67" s="2"/>
+      <c r="G67" s="2"/>
+      <c r="H67" s="2"/>
+      <c r="I67" s="2"/>
+      <c r="J67" s="2"/>
+      <c r="K67" s="2"/>
+      <c r="L67" s="2"/>
+      <c r="M67" s="2"/>
+      <c r="N67" s="2"/>
+      <c r="O67" s="2"/>
+      <c r="P67" s="5"/>
+      <c r="Q67" s="6"/>
+      <c r="R67" s="6"/>
+      <c r="S67" s="6"/>
+      <c r="T67" s="6"/>
+      <c r="U67" s="6"/>
+      <c r="V67" s="6"/>
+      <c r="W67" s="6"/>
+      <c r="X67" s="6"/>
+      <c r="Y67" s="6"/>
+      <c r="Z67" s="6"/>
     </row>
     <row r="68" spans="5:26" x14ac:dyDescent="0.2">
-      <c r="E68" s="2">
-        <v>10</v>
-      </c>
-      <c r="F68" s="2">
-        <v>1000</v>
-      </c>
-      <c r="G68" s="2">
-        <v>0.4</v>
-      </c>
-      <c r="H68" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="I68" s="2">
-        <v>50</v>
-      </c>
-      <c r="J68" s="2">
-        <v>1000</v>
-      </c>
-      <c r="K68" s="2">
-        <v>56665</v>
-      </c>
-      <c r="L68" s="2">
-        <v>9072</v>
-      </c>
-      <c r="M68" s="2">
-        <v>26</v>
-      </c>
-      <c r="N68" s="2">
-        <v>50507.882812000003</v>
-      </c>
-      <c r="O68" s="2">
-        <v>5.1500000000000005E-4</v>
-      </c>
-      <c r="P68" s="5">
-        <v>10</v>
-      </c>
-      <c r="Q68" s="6">
-        <v>1000</v>
-      </c>
-      <c r="R68" s="6">
-        <v>0.6</v>
-      </c>
-      <c r="S68" s="6">
-        <v>0.2</v>
-      </c>
-      <c r="T68" s="6">
-        <v>50</v>
-      </c>
-      <c r="U68" s="6">
-        <v>1000</v>
-      </c>
-      <c r="V68" s="6">
-        <v>69019</v>
-      </c>
-      <c r="W68" s="6">
-        <v>8988</v>
-      </c>
-      <c r="X68" s="6">
-        <v>29</v>
-      </c>
-      <c r="Y68" s="6">
-        <v>49900.113280999998</v>
-      </c>
-      <c r="Z68" s="6">
-        <v>5.8100000000000003E-4</v>
-      </c>
+      <c r="E68" s="2"/>
+      <c r="F68" s="2"/>
+      <c r="G68" s="2"/>
+      <c r="H68" s="2"/>
+      <c r="I68" s="2"/>
+      <c r="J68" s="2"/>
+      <c r="K68" s="2"/>
+      <c r="L68" s="2"/>
+      <c r="M68" s="2"/>
+      <c r="N68" s="2"/>
+      <c r="O68" s="2"/>
+      <c r="P68" s="5"/>
+      <c r="Q68" s="6"/>
+      <c r="R68" s="6"/>
+      <c r="S68" s="6"/>
+      <c r="T68" s="6"/>
+      <c r="U68" s="6"/>
+      <c r="V68" s="6"/>
+      <c r="W68" s="6"/>
+      <c r="X68" s="6"/>
+      <c r="Y68" s="6"/>
+      <c r="Z68" s="6"/>
     </row>
     <row r="69" spans="5:26" x14ac:dyDescent="0.2">
       <c r="E69" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="F69" s="2">
+      <c r="F69" s="2" t="e">
         <f>AVERAGE(F59:F68)</f>
-        <v>1000</v>
-      </c>
-      <c r="G69" s="2">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G69" s="2" t="e">
         <f t="shared" ref="G69:O69" si="9">AVERAGE(G59:G68)</f>
-        <v>0.39999999999999997</v>
-      </c>
-      <c r="H69" s="2">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H69" s="2" t="e">
         <f t="shared" si="9"/>
-        <v>0.19999999999999998</v>
-      </c>
-      <c r="I69" s="2">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I69" s="2" t="e">
         <f t="shared" si="9"/>
-        <v>50</v>
-      </c>
-      <c r="J69" s="2">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J69" s="2" t="e">
         <f t="shared" si="9"/>
-        <v>1000</v>
-      </c>
-      <c r="K69" s="2">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K69" s="2" t="e">
         <f t="shared" si="9"/>
-        <v>48191.9</v>
-      </c>
-      <c r="L69" s="2">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L69" s="2" t="e">
         <f t="shared" si="9"/>
-        <v>9029.4</v>
-      </c>
-      <c r="M69" s="2">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M69" s="2" t="e">
         <f t="shared" si="9"/>
-        <v>24.4</v>
-      </c>
-      <c r="N69" s="2">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N69" s="2" t="e">
         <f t="shared" si="9"/>
-        <v>49951.421874899999</v>
-      </c>
-      <c r="O69" s="2">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O69" s="2" t="e">
         <f t="shared" si="9"/>
-        <v>4.8790000000000004E-4</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="P69" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="Q69" s="6">
+      <c r="Q69" s="6" t="e">
         <f>AVERAGE(Q59:Q68)</f>
-        <v>1000</v>
-      </c>
-      <c r="R69" s="6">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R69" s="6" t="e">
         <f t="shared" ref="R69:Z69" si="10">AVERAGE(R59:R68)</f>
-        <v>0.59999999999999987</v>
-      </c>
-      <c r="S69" s="6">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S69" s="6" t="e">
         <f t="shared" si="10"/>
-        <v>0.19999999999999998</v>
-      </c>
-      <c r="T69" s="6">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T69" s="6" t="e">
         <f t="shared" si="10"/>
-        <v>50</v>
-      </c>
-      <c r="U69" s="6">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U69" s="6" t="e">
         <f t="shared" si="10"/>
-        <v>1000</v>
-      </c>
-      <c r="V69" s="6">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V69" s="6" t="e">
         <f t="shared" si="10"/>
-        <v>53798.5</v>
-      </c>
-      <c r="W69" s="6">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="W69" s="6" t="e">
         <f t="shared" si="10"/>
-        <v>9026.5</v>
-      </c>
-      <c r="X69" s="6">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="X69" s="6" t="e">
         <f t="shared" si="10"/>
-        <v>24.3</v>
-      </c>
-      <c r="Y69" s="6">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Y69" s="6" t="e">
         <f t="shared" si="10"/>
-        <v>49847.908203300001</v>
-      </c>
-      <c r="Z69" s="6">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Z69" s="6" t="e">
         <f t="shared" si="10"/>
-        <v>4.885E-4</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="70" spans="5:26" x14ac:dyDescent="0.2">
@@ -6843,433 +6269,191 @@
       <c r="O98" s="16"/>
     </row>
     <row r="99" spans="5:15" x14ac:dyDescent="0.2">
-      <c r="E99" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="F99" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="G99" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="H99" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="I99" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="J99" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="K99" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="L99" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="M99" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="N99" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="O99" s="6" t="s">
-        <v>10</v>
-      </c>
+      <c r="E99" s="5"/>
+      <c r="F99" s="6"/>
+      <c r="G99" s="6"/>
+      <c r="H99" s="6"/>
+      <c r="I99" s="6"/>
+      <c r="J99" s="6"/>
+      <c r="K99" s="6"/>
+      <c r="L99" s="6"/>
+      <c r="M99" s="6"/>
+      <c r="N99" s="6"/>
+      <c r="O99" s="6"/>
     </row>
     <row r="100" spans="5:15" x14ac:dyDescent="0.2">
-      <c r="E100" s="5">
-        <v>1</v>
-      </c>
-      <c r="F100" s="6">
-        <v>1000</v>
-      </c>
-      <c r="G100" s="6">
-        <v>0.8</v>
-      </c>
-      <c r="H100" s="6">
-        <v>0.2</v>
-      </c>
-      <c r="I100" s="6">
-        <v>50</v>
-      </c>
-      <c r="J100" s="6">
-        <v>1000</v>
-      </c>
-      <c r="K100" s="6">
-        <v>32963</v>
-      </c>
-      <c r="L100" s="6">
-        <v>6658</v>
-      </c>
-      <c r="M100" s="6">
-        <v>10</v>
-      </c>
-      <c r="N100" s="6">
-        <v>49779.804687999997</v>
-      </c>
-      <c r="O100" s="6">
-        <v>2.0100000000000001E-4</v>
-      </c>
+      <c r="E100" s="5"/>
+      <c r="F100" s="6"/>
+      <c r="G100" s="6"/>
+      <c r="H100" s="6"/>
+      <c r="I100" s="6"/>
+      <c r="J100" s="6"/>
+      <c r="K100" s="6"/>
+      <c r="L100" s="6"/>
+      <c r="M100" s="6"/>
+      <c r="N100" s="6"/>
+      <c r="O100" s="6"/>
     </row>
     <row r="101" spans="5:15" x14ac:dyDescent="0.2">
-      <c r="E101" s="5">
-        <v>2</v>
-      </c>
-      <c r="F101" s="6">
-        <v>1000</v>
-      </c>
-      <c r="G101" s="6">
-        <v>0.8</v>
-      </c>
-      <c r="H101" s="6">
-        <v>0.2</v>
-      </c>
-      <c r="I101" s="6">
-        <v>50</v>
-      </c>
-      <c r="J101" s="6">
-        <v>1000</v>
-      </c>
-      <c r="K101" s="6">
-        <v>46513</v>
-      </c>
-      <c r="L101" s="6">
-        <v>9031</v>
-      </c>
-      <c r="M101" s="6">
-        <v>10</v>
-      </c>
-      <c r="N101" s="6">
-        <v>50142.882812000003</v>
-      </c>
-      <c r="O101" s="6">
-        <v>1.9900000000000001E-4</v>
-      </c>
+      <c r="E101" s="5"/>
+      <c r="F101" s="6"/>
+      <c r="G101" s="6"/>
+      <c r="H101" s="6"/>
+      <c r="I101" s="6"/>
+      <c r="J101" s="6"/>
+      <c r="K101" s="6"/>
+      <c r="L101" s="6"/>
+      <c r="M101" s="6"/>
+      <c r="N101" s="6"/>
+      <c r="O101" s="6"/>
     </row>
     <row r="102" spans="5:15" x14ac:dyDescent="0.2">
-      <c r="E102" s="5">
-        <v>3</v>
-      </c>
-      <c r="F102" s="6">
-        <v>1000</v>
-      </c>
-      <c r="G102" s="6">
-        <v>0.8</v>
-      </c>
-      <c r="H102" s="6">
-        <v>0.2</v>
-      </c>
-      <c r="I102" s="6">
-        <v>50</v>
-      </c>
-      <c r="J102" s="6">
-        <v>1000</v>
-      </c>
-      <c r="K102" s="6">
-        <v>32623</v>
-      </c>
-      <c r="L102" s="6">
-        <v>6456</v>
-      </c>
-      <c r="M102" s="6">
-        <v>10</v>
-      </c>
-      <c r="N102" s="6">
-        <v>49229.574219000002</v>
-      </c>
-      <c r="O102" s="6">
-        <v>2.03E-4</v>
-      </c>
+      <c r="E102" s="5"/>
+      <c r="F102" s="6"/>
+      <c r="G102" s="6"/>
+      <c r="H102" s="6"/>
+      <c r="I102" s="6"/>
+      <c r="J102" s="6"/>
+      <c r="K102" s="6"/>
+      <c r="L102" s="6"/>
+      <c r="M102" s="6"/>
+      <c r="N102" s="6"/>
+      <c r="O102" s="6"/>
     </row>
     <row r="103" spans="5:15" x14ac:dyDescent="0.2">
-      <c r="E103" s="5">
-        <v>4</v>
-      </c>
-      <c r="F103" s="6">
-        <v>1000</v>
-      </c>
-      <c r="G103" s="6">
-        <v>0.8</v>
-      </c>
-      <c r="H103" s="6">
-        <v>0.2</v>
-      </c>
-      <c r="I103" s="6">
-        <v>50</v>
-      </c>
-      <c r="J103" s="6">
-        <v>1000</v>
-      </c>
-      <c r="K103" s="6">
-        <v>36018</v>
-      </c>
-      <c r="L103" s="6">
-        <v>7190</v>
-      </c>
-      <c r="M103" s="6">
-        <v>12</v>
-      </c>
-      <c r="N103" s="6">
-        <v>49526.425780999998</v>
-      </c>
-      <c r="O103" s="6">
-        <v>2.42E-4</v>
-      </c>
+      <c r="E103" s="5"/>
+      <c r="F103" s="6"/>
+      <c r="G103" s="6"/>
+      <c r="H103" s="6"/>
+      <c r="I103" s="6"/>
+      <c r="J103" s="6"/>
+      <c r="K103" s="6"/>
+      <c r="L103" s="6"/>
+      <c r="M103" s="6"/>
+      <c r="N103" s="6"/>
+      <c r="O103" s="6"/>
     </row>
     <row r="104" spans="5:15" x14ac:dyDescent="0.2">
-      <c r="E104" s="5">
-        <v>5</v>
-      </c>
-      <c r="F104" s="6">
-        <v>1000</v>
-      </c>
-      <c r="G104" s="6">
-        <v>0.8</v>
-      </c>
-      <c r="H104" s="6">
-        <v>0.2</v>
-      </c>
-      <c r="I104" s="6">
-        <v>50</v>
-      </c>
-      <c r="J104" s="6">
-        <v>1000</v>
-      </c>
-      <c r="K104" s="6">
-        <v>49654</v>
-      </c>
-      <c r="L104" s="6">
-        <v>8987</v>
-      </c>
-      <c r="M104" s="6">
-        <v>18</v>
-      </c>
-      <c r="N104" s="6">
-        <v>50165.960937999997</v>
-      </c>
-      <c r="O104" s="6">
-        <v>3.59E-4</v>
-      </c>
+      <c r="E104" s="5"/>
+      <c r="F104" s="6"/>
+      <c r="G104" s="6"/>
+      <c r="H104" s="6"/>
+      <c r="I104" s="6"/>
+      <c r="J104" s="6"/>
+      <c r="K104" s="6"/>
+      <c r="L104" s="6"/>
+      <c r="M104" s="6"/>
+      <c r="N104" s="6"/>
+      <c r="O104" s="6"/>
     </row>
     <row r="105" spans="5:15" x14ac:dyDescent="0.2">
-      <c r="E105" s="5">
-        <v>6</v>
-      </c>
-      <c r="F105" s="6">
-        <v>1000</v>
-      </c>
-      <c r="G105" s="6">
-        <v>0.8</v>
-      </c>
-      <c r="H105" s="6">
-        <v>0.2</v>
-      </c>
-      <c r="I105" s="6">
-        <v>50</v>
-      </c>
-      <c r="J105" s="6">
-        <v>1000</v>
-      </c>
-      <c r="K105" s="6">
-        <v>59875</v>
-      </c>
-      <c r="L105" s="6">
-        <v>9162</v>
-      </c>
-      <c r="M105" s="6">
-        <v>19</v>
-      </c>
-      <c r="N105" s="6">
-        <v>50725.347655999998</v>
-      </c>
-      <c r="O105" s="6">
-        <v>3.7500000000000001E-4</v>
-      </c>
+      <c r="E105" s="5"/>
+      <c r="F105" s="6"/>
+      <c r="G105" s="6"/>
+      <c r="H105" s="6"/>
+      <c r="I105" s="6"/>
+      <c r="J105" s="6"/>
+      <c r="K105" s="6"/>
+      <c r="L105" s="6"/>
+      <c r="M105" s="6"/>
+      <c r="N105" s="6"/>
+      <c r="O105" s="6"/>
     </row>
     <row r="106" spans="5:15" x14ac:dyDescent="0.2">
-      <c r="E106" s="5">
-        <v>7</v>
-      </c>
-      <c r="F106" s="6">
-        <v>1000</v>
-      </c>
-      <c r="G106" s="6">
-        <v>0.8</v>
-      </c>
-      <c r="H106" s="6">
-        <v>0.2</v>
-      </c>
-      <c r="I106" s="6">
-        <v>50</v>
-      </c>
-      <c r="J106" s="6">
-        <v>1000</v>
-      </c>
-      <c r="K106" s="6">
-        <v>43133</v>
-      </c>
-      <c r="L106" s="6">
-        <v>8516</v>
-      </c>
-      <c r="M106" s="6">
-        <v>14</v>
-      </c>
-      <c r="N106" s="6">
-        <v>50198.304687999997</v>
-      </c>
-      <c r="O106" s="6">
-        <v>2.7900000000000001E-4</v>
-      </c>
+      <c r="E106" s="5"/>
+      <c r="F106" s="6"/>
+      <c r="G106" s="6"/>
+      <c r="H106" s="6"/>
+      <c r="I106" s="6"/>
+      <c r="J106" s="6"/>
+      <c r="K106" s="6"/>
+      <c r="L106" s="6"/>
+      <c r="M106" s="6"/>
+      <c r="N106" s="6"/>
+      <c r="O106" s="6"/>
     </row>
     <row r="107" spans="5:15" x14ac:dyDescent="0.2">
-      <c r="E107" s="5">
-        <v>8</v>
-      </c>
-      <c r="F107" s="6">
-        <v>1000</v>
-      </c>
-      <c r="G107" s="6">
-        <v>0.8</v>
-      </c>
-      <c r="H107" s="6">
-        <v>0.2</v>
-      </c>
-      <c r="I107" s="6">
-        <v>50</v>
-      </c>
-      <c r="J107" s="6">
-        <v>1000</v>
-      </c>
-      <c r="K107" s="6">
-        <v>49331</v>
-      </c>
-      <c r="L107" s="6">
-        <v>9018</v>
-      </c>
-      <c r="M107" s="6">
-        <v>15</v>
-      </c>
-      <c r="N107" s="6">
-        <v>49778.015625</v>
-      </c>
-      <c r="O107" s="6">
-        <v>3.01E-4</v>
-      </c>
+      <c r="E107" s="5"/>
+      <c r="F107" s="6"/>
+      <c r="G107" s="6"/>
+      <c r="H107" s="6"/>
+      <c r="I107" s="6"/>
+      <c r="J107" s="6"/>
+      <c r="K107" s="6"/>
+      <c r="L107" s="6"/>
+      <c r="M107" s="6"/>
+      <c r="N107" s="6"/>
+      <c r="O107" s="6"/>
     </row>
     <row r="108" spans="5:15" x14ac:dyDescent="0.2">
-      <c r="E108" s="5">
-        <v>9</v>
-      </c>
-      <c r="F108" s="6">
-        <v>1000</v>
-      </c>
-      <c r="G108" s="6">
-        <v>0.8</v>
-      </c>
-      <c r="H108" s="6">
-        <v>0.2</v>
-      </c>
-      <c r="I108" s="6">
-        <v>50</v>
-      </c>
-      <c r="J108" s="6">
-        <v>1000</v>
-      </c>
-      <c r="K108" s="6">
-        <v>68341</v>
-      </c>
-      <c r="L108" s="6">
-        <v>8909</v>
-      </c>
-      <c r="M108" s="6">
-        <v>26</v>
-      </c>
-      <c r="N108" s="6">
-        <v>49524.308594000002</v>
-      </c>
-      <c r="O108" s="6">
-        <v>5.2499999999999997E-4</v>
-      </c>
+      <c r="E108" s="5"/>
+      <c r="F108" s="6"/>
+      <c r="G108" s="6"/>
+      <c r="H108" s="6"/>
+      <c r="I108" s="6"/>
+      <c r="J108" s="6"/>
+      <c r="K108" s="6"/>
+      <c r="L108" s="6"/>
+      <c r="M108" s="6"/>
+      <c r="N108" s="6"/>
+      <c r="O108" s="6"/>
     </row>
     <row r="109" spans="5:15" x14ac:dyDescent="0.2">
-      <c r="E109" s="5">
-        <v>10</v>
-      </c>
-      <c r="F109" s="6">
-        <v>1000</v>
-      </c>
-      <c r="G109" s="6">
-        <v>0.8</v>
-      </c>
-      <c r="H109" s="6">
-        <v>0.2</v>
-      </c>
-      <c r="I109" s="6">
-        <v>50</v>
-      </c>
-      <c r="J109" s="6">
-        <v>1000</v>
-      </c>
-      <c r="K109" s="6">
-        <v>29292</v>
-      </c>
-      <c r="L109" s="6">
-        <v>5848</v>
-      </c>
-      <c r="M109" s="6">
-        <v>10</v>
-      </c>
-      <c r="N109" s="6">
-        <v>49057.261719000002</v>
-      </c>
-      <c r="O109" s="6">
-        <v>2.04E-4</v>
-      </c>
+      <c r="E109" s="5"/>
+      <c r="F109" s="6"/>
+      <c r="G109" s="6"/>
+      <c r="H109" s="6"/>
+      <c r="I109" s="6"/>
+      <c r="J109" s="6"/>
+      <c r="K109" s="6"/>
+      <c r="L109" s="6"/>
+      <c r="M109" s="6"/>
+      <c r="N109" s="6"/>
+      <c r="O109" s="6"/>
     </row>
     <row r="110" spans="5:15" x14ac:dyDescent="0.2">
       <c r="E110" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="F110" s="6">
+      <c r="F110" s="6" t="e">
         <f>AVERAGE(F100:F109)</f>
-        <v>1000</v>
-      </c>
-      <c r="G110" s="6">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G110" s="6" t="e">
         <f t="shared" ref="G110:O110" si="14">AVERAGE(G100:G109)</f>
-        <v>0.79999999999999993</v>
-      </c>
-      <c r="H110" s="6">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H110" s="6" t="e">
         <f t="shared" si="14"/>
-        <v>0.19999999999999998</v>
-      </c>
-      <c r="I110" s="6">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I110" s="6" t="e">
         <f t="shared" si="14"/>
-        <v>50</v>
-      </c>
-      <c r="J110" s="6">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J110" s="6" t="e">
         <f t="shared" si="14"/>
-        <v>1000</v>
-      </c>
-      <c r="K110" s="6">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K110" s="6" t="e">
         <f t="shared" si="14"/>
-        <v>44774.3</v>
-      </c>
-      <c r="L110" s="6">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L110" s="6" t="e">
         <f t="shared" si="14"/>
-        <v>7977.5</v>
-      </c>
-      <c r="M110" s="6">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M110" s="6" t="e">
         <f t="shared" si="14"/>
-        <v>14.4</v>
-      </c>
-      <c r="N110" s="6">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N110" s="6" t="e">
         <f t="shared" si="14"/>
-        <v>49812.788672000002</v>
-      </c>
-      <c r="O110" s="6">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O110" s="6" t="e">
         <f t="shared" si="14"/>
-        <v>2.8879999999999997E-4</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="111" spans="5:15" x14ac:dyDescent="0.2">
@@ -7748,8 +6932,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V123"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="75" workbookViewId="0">
-      <selection activeCell="R51" sqref="R51"/>
+    <sheetView topLeftCell="A5" zoomScale="125" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17:N27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7762,7 +6946,7 @@
     <col min="6" max="6" width="12.5" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="11.1640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10" customWidth="1"/>
+    <col min="10" max="10" width="15.6640625" customWidth="1"/>
     <col min="12" max="12" width="4.83203125" customWidth="1"/>
     <col min="13" max="13" width="9" customWidth="1"/>
     <col min="14" max="14" width="4.5" customWidth="1"/>
@@ -7771,7 +6955,7 @@
     <col min="17" max="17" width="12.5" bestFit="1" customWidth="1"/>
     <col min="18" max="19" width="11.1640625" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="10" customWidth="1"/>
+    <col min="21" max="21" width="26.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Tweak GBN timeout scheme; Update experiments
</commit_message>
<xml_diff>
--- a/scripts/Experiment 1 Results/Experiment 1 Graphs.xlsx
+++ b/scripts/Experiment 1 Results/Experiment 1 Graphs.xlsx
@@ -7758,8 +7758,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="L1:AG123"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H69" zoomScale="82" workbookViewId="0">
-      <selection activeCell="L99" sqref="L99:V109"/>
+    <sheetView tabSelected="1" topLeftCell="F77" zoomScale="82" workbookViewId="0">
+      <selection activeCell="V110" sqref="V110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -12212,11 +12212,11 @@
         <v>134.6</v>
       </c>
       <c r="AF69" s="6">
-        <f t="shared" ref="AF69" si="72">AVERAGE(AF59:AF68)</f>
+        <f t="shared" ref="AF69:AG69" si="72">AVERAGE(AF59:AF68)</f>
         <v>50418.996875099998</v>
       </c>
       <c r="AG69" s="6">
-        <f t="shared" ref="AG69" si="73">AVERAGE(AG59:AG68)</f>
+        <f t="shared" si="72"/>
         <v>2.6713000000000002E-3</v>
       </c>
     </row>
@@ -13005,39 +13005,39 @@
         <v>1000</v>
       </c>
       <c r="N82" s="6">
-        <f t="shared" ref="N82" si="74">AVERAGE(N72:N81)</f>
+        <f t="shared" ref="N82" si="73">AVERAGE(N72:N81)</f>
         <v>0.39999999999999997</v>
       </c>
       <c r="O82" s="6">
-        <f t="shared" ref="O82" si="75">AVERAGE(O72:O81)</f>
+        <f t="shared" ref="O82" si="74">AVERAGE(O72:O81)</f>
         <v>0.19999999999999998</v>
       </c>
       <c r="P82" s="6">
-        <f t="shared" ref="P82" si="76">AVERAGE(P72:P81)</f>
+        <f t="shared" ref="P82" si="75">AVERAGE(P72:P81)</f>
         <v>50</v>
       </c>
       <c r="Q82" s="6">
-        <f t="shared" ref="Q82" si="77">AVERAGE(Q72:Q81)</f>
+        <f t="shared" ref="Q82" si="76">AVERAGE(Q72:Q81)</f>
         <v>1000</v>
       </c>
       <c r="R82" s="6">
-        <f t="shared" ref="R82" si="78">AVERAGE(R72:R81)</f>
+        <f t="shared" ref="R82" si="77">AVERAGE(R72:R81)</f>
         <v>1501</v>
       </c>
       <c r="S82" s="6">
-        <f t="shared" ref="S82" si="79">AVERAGE(S72:S81)</f>
+        <f t="shared" ref="S82" si="78">AVERAGE(S72:S81)</f>
         <v>901</v>
       </c>
       <c r="T82" s="6">
-        <f t="shared" ref="T82" si="80">AVERAGE(T72:T81)</f>
+        <f t="shared" ref="T82" si="79">AVERAGE(T72:T81)</f>
         <v>9.6999999999999993</v>
       </c>
       <c r="U82" s="6">
-        <f t="shared" ref="U82" si="81">AVERAGE(U72:U81)</f>
+        <f t="shared" ref="U82" si="80">AVERAGE(U72:U81)</f>
         <v>50103.7</v>
       </c>
       <c r="V82" s="6">
-        <f t="shared" ref="V82" si="82">AVERAGE(V72:V81)</f>
+        <f t="shared" ref="V82" si="81">AVERAGE(V72:V81)</f>
         <v>1.9500000000000002E-4</v>
       </c>
       <c r="W82" s="3" t="s">
@@ -13048,39 +13048,39 @@
         <v>1000</v>
       </c>
       <c r="Y82" s="6">
-        <f t="shared" ref="Y82" si="83">AVERAGE(Y72:Y81)</f>
+        <f t="shared" ref="Y82" si="82">AVERAGE(Y72:Y81)</f>
         <v>0.59999999999999987</v>
       </c>
       <c r="Z82" s="6">
-        <f t="shared" ref="Z82" si="84">AVERAGE(Z72:Z81)</f>
+        <f t="shared" ref="Z82" si="83">AVERAGE(Z72:Z81)</f>
         <v>0.19999999999999998</v>
       </c>
       <c r="AA82" s="6">
-        <f t="shared" ref="AA82" si="85">AVERAGE(AA72:AA81)</f>
+        <f t="shared" ref="AA82" si="84">AVERAGE(AA72:AA81)</f>
         <v>50</v>
       </c>
       <c r="AB82" s="6">
-        <f t="shared" ref="AB82" si="86">AVERAGE(AB72:AB81)</f>
+        <f t="shared" ref="AB82" si="85">AVERAGE(AB72:AB81)</f>
         <v>1000</v>
       </c>
       <c r="AC82" s="6">
-        <f t="shared" ref="AC82" si="87">AVERAGE(AC72:AC81)</f>
+        <f t="shared" ref="AC82" si="86">AVERAGE(AC72:AC81)</f>
         <v>63546.5</v>
       </c>
       <c r="AD82" s="6">
-        <f t="shared" ref="AD82" si="88">AVERAGE(AD72:AD81)</f>
+        <f t="shared" ref="AD82" si="87">AVERAGE(AD72:AD81)</f>
         <v>4356.6000000000004</v>
       </c>
       <c r="AE82" s="6">
-        <f t="shared" ref="AE82" si="89">AVERAGE(AE72:AE81)</f>
+        <f t="shared" ref="AE82" si="88">AVERAGE(AE72:AE81)</f>
         <v>8.5</v>
       </c>
       <c r="AF82" s="6">
-        <f t="shared" ref="AF82" si="90">AVERAGE(AF72:AF81)</f>
+        <f t="shared" ref="AF82" si="89">AVERAGE(AF72:AF81)</f>
         <v>49956.1</v>
       </c>
       <c r="AG82" s="6">
-        <f t="shared" ref="AG82" si="91">AVERAGE(AG72:AG81)</f>
+        <f t="shared" ref="AG82" si="90">AVERAGE(AG72:AG81)</f>
         <v>1.7019999999999999E-4</v>
       </c>
     </row>
@@ -13521,39 +13521,39 @@
         <v>1000</v>
       </c>
       <c r="N97" s="6">
-        <f t="shared" ref="N97:V97" si="92">AVERAGE(N87:N96)</f>
+        <f t="shared" ref="N97:V97" si="91">AVERAGE(N87:N96)</f>
         <v>0.79999999999999993</v>
       </c>
       <c r="O97" s="6">
-        <f t="shared" si="92"/>
+        <f t="shared" si="91"/>
         <v>0.19999999999999998</v>
       </c>
       <c r="P97" s="6">
-        <f t="shared" si="92"/>
+        <f t="shared" si="91"/>
         <v>50</v>
       </c>
       <c r="Q97" s="6">
-        <f t="shared" si="92"/>
+        <f t="shared" si="91"/>
         <v>1000</v>
       </c>
       <c r="R97" s="6">
-        <f t="shared" si="92"/>
+        <f t="shared" si="91"/>
         <v>4621.3999999999996</v>
       </c>
       <c r="S97" s="6">
-        <f t="shared" si="92"/>
+        <f t="shared" si="91"/>
         <v>934.9</v>
       </c>
       <c r="T97" s="6">
-        <f t="shared" si="92"/>
+        <f t="shared" si="91"/>
         <v>119.1</v>
       </c>
       <c r="U97" s="6">
-        <f t="shared" si="92"/>
+        <f t="shared" si="91"/>
         <v>49768.623437599999</v>
       </c>
       <c r="V97" s="6">
-        <f t="shared" si="92"/>
+        <f t="shared" si="91"/>
         <v>2.3927999999999996E-3</v>
       </c>
     </row>
@@ -13966,39 +13966,39 @@
         <v>1000</v>
       </c>
       <c r="N110" s="6">
-        <f t="shared" ref="N110:U110" si="93">AVERAGE(N100:N109)</f>
+        <f t="shared" ref="N110:V110" si="92">AVERAGE(N100:N109)</f>
         <v>0.79999999999999993</v>
       </c>
       <c r="O110" s="6">
-        <f t="shared" si="93"/>
+        <f t="shared" si="92"/>
         <v>0.19999999999999998</v>
       </c>
       <c r="P110" s="6">
-        <f t="shared" si="93"/>
+        <f t="shared" si="92"/>
         <v>50</v>
       </c>
       <c r="Q110" s="6">
-        <f t="shared" si="93"/>
+        <f t="shared" si="92"/>
         <v>1000</v>
       </c>
       <c r="R110" s="6">
-        <f t="shared" si="93"/>
+        <f t="shared" si="92"/>
         <v>463.4</v>
       </c>
       <c r="S110" s="6">
-        <f t="shared" si="93"/>
+        <f t="shared" si="92"/>
         <v>94.8</v>
       </c>
       <c r="T110" s="6">
-        <f t="shared" si="93"/>
+        <f t="shared" si="92"/>
         <v>5.0999999999999996</v>
       </c>
       <c r="U110" s="6">
-        <f t="shared" si="93"/>
+        <f t="shared" si="92"/>
         <v>49974.130468900003</v>
       </c>
       <c r="V110" s="6">
-        <f>AVERAGE(V100:V109)</f>
+        <f t="shared" si="92"/>
         <v>1.0180000000000001E-4</v>
       </c>
     </row>
@@ -14411,35 +14411,35 @@
         <v>1000</v>
       </c>
       <c r="N123" s="6">
-        <f t="shared" ref="N123:U123" si="94">AVERAGE(N113:N122)</f>
+        <f t="shared" ref="N123:U123" si="93">AVERAGE(N113:N122)</f>
         <v>0.79999999999999993</v>
       </c>
       <c r="O123" s="6">
-        <f t="shared" si="94"/>
+        <f t="shared" si="93"/>
         <v>0.19999999999999998</v>
       </c>
       <c r="P123" s="6">
-        <f t="shared" si="94"/>
+        <f t="shared" si="93"/>
         <v>50</v>
       </c>
       <c r="Q123" s="6">
-        <f t="shared" si="94"/>
+        <f t="shared" si="93"/>
         <v>1000</v>
       </c>
       <c r="R123" s="6">
-        <f t="shared" si="94"/>
+        <f t="shared" si="93"/>
         <v>140671.6</v>
       </c>
       <c r="S123" s="6">
-        <f t="shared" si="94"/>
+        <f t="shared" si="93"/>
         <v>8124.7</v>
       </c>
       <c r="T123" s="6">
-        <f t="shared" si="94"/>
+        <f t="shared" si="93"/>
         <v>7.3</v>
       </c>
       <c r="U123" s="6">
-        <f t="shared" si="94"/>
+        <f t="shared" si="93"/>
         <v>50274.400000000001</v>
       </c>
       <c r="V123" s="6">

</xml_diff>